<commit_message>
Added final pdfs to project
</commit_message>
<xml_diff>
--- a/Star Assault Testing.xlsx
+++ b/Star Assault Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galwaymayoinstitute-my.sharepoint.com/personal/g00363458_gmit_ie/Documents/Desktop/StarAsault/Final-year-MAD3-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="13_ncr:1_{D99A2A5C-765B-448C-BFE6-16FA8DE1C7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6BBE30A8-ACA8-41D9-8E7B-6964407D0453}"/>
+  <xr:revisionPtr revIDLastSave="529" documentId="13_ncr:1_{D99A2A5C-765B-448C-BFE6-16FA8DE1C7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E09E1D1-F9D7-40A1-BABD-B03FF976D598}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="193">
   <si>
     <t>Project Name</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>To be assigned</t>
   </si>
   <si>
     <t>Test Case Name</t>
@@ -491,12 +488,6 @@
     <t>In Game Menus</t>
   </si>
   <si>
-    <t>Launch Settings Menu</t>
-  </si>
-  <si>
-    <t>If volume can be changed and sound turned on and off</t>
-  </si>
-  <si>
     <t>Game pauses when esc is pressed,  the game will  reusme when resume button is clicked, or esc button is clicked again</t>
   </si>
   <si>
@@ -576,6 +567,80 @@
   </si>
   <si>
     <t>Not working</t>
+  </si>
+  <si>
+    <t>TC.038</t>
+  </si>
+  <si>
+    <t>TC.039</t>
+  </si>
+  <si>
+    <t>Launch Game Begin scene</t>
+  </si>
+  <si>
+    <t>If sound on/off works</t>
+  </si>
+  <si>
+    <t>When player selects sound icon the sound mutes/unmutes</t>
+  </si>
+  <si>
+    <t>sound mutes as expected</t>
+  </si>
+  <si>
+    <t>Launch level 1</t>
+  </si>
+  <si>
+    <t>sound mutes but  when player fires a bullet this also mutes/unmutes sound</t>
+  </si>
+  <si>
+    <t>Multiplayer game works</t>
+  </si>
+  <si>
+    <t>Multiplayer game starts</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t>Defect No 00008
+Priority-4
+Severity-Minor</t>
+  </si>
+  <si>
+    <t>Defect No 00009
+Priority-4
+Severity-Minor</t>
+  </si>
+  <si>
+    <t>Defect No 00010
+Priority-4
+Severity-Minor</t>
+  </si>
+  <si>
+    <t>Defect No 00011
+Priority-4
+Severity-Minor</t>
+  </si>
+  <si>
+    <t>Defect No 00012
+Priority-4
+Severity-Minor</t>
+  </si>
+  <si>
+    <t>Defect No 00013
+Priority-2
+Severity-Major</t>
+  </si>
+  <si>
+    <t>Defect No 00014
+Priority-2
+Severity-Major</t>
+  </si>
+  <si>
+    <t>Shirin</t>
+  </si>
+  <si>
+    <t>More senior developer</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1179,9 +1244,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1222,9 +1284,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1296,12 +1355,48 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1873,9 +1968,9 @@
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1905,11 +2000,11 @@
     <row r="6" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1918,10 +2013,10 @@
       <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="66"/>
+      <c r="E7" s="64"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1930,10 +2025,10 @@
       <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="68"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1958,10 +2053,10 @@
       <c r="C11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="70"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1970,10 +2065,10 @@
       <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="72"/>
+      <c r="E12" s="70"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1982,8 +2077,8 @@
       <c r="C13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2021,11 +2116,11 @@
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2065,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>9</v>
@@ -2290,104 +2385,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67821BE3-FC89-4E7A-A2B7-8A4F8B0D7E8B}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="45" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="47" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="42" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="41" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="70.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44"/>
+      <c r="A1" s="43"/>
       <c r="B1" s="35"/>
       <c r="C1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="73"/>
+      <c r="D1" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="71"/>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
-      <c r="J1" s="40"/>
+      <c r="J1" s="39"/>
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="76"/>
+      <c r="A2" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="74"/>
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
-      <c r="J2" s="41"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="51" t="s">
+      <c r="D3" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="51" t="s">
+      <c r="F3" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="50" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45">
+      <c r="A4" s="44">
         <v>1</v>
       </c>
       <c r="B4" s="33">
@@ -2397,31 +2492,31 @@
         <v>24</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="H4" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="48" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
+      <c r="A5" s="44">
         <v>1.1000000000000001</v>
       </c>
       <c r="B5" s="33">
@@ -2431,31 +2526,31 @@
         <v>27</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>71</v>
-      </c>
       <c r="I5" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="48" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
+      <c r="A6" s="44">
         <v>1.2</v>
       </c>
       <c r="B6" s="33">
@@ -2465,1198 +2560,1308 @@
         <v>28</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>64</v>
-      </c>
       <c r="I6" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="33"/>
     </row>
     <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="45">
+      <c r="A7" s="44">
         <v>1.3</v>
       </c>
       <c r="B7" s="33">
         <v>1</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="I7" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="34"/>
       <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
+      <c r="A8" s="44">
         <v>1.3</v>
       </c>
       <c r="B8" s="33">
         <v>1</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="I8" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="34"/>
       <c r="L8" s="33"/>
     </row>
     <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="45">
+      <c r="A9" s="44">
         <v>2</v>
       </c>
       <c r="B9" s="33">
         <v>1</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G9" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="I9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="34"/>
       <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
+      <c r="A10" s="44">
         <v>2.1</v>
       </c>
       <c r="B10" s="33">
         <v>1</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="I10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K10" s="34"/>
       <c r="L10" s="33"/>
     </row>
     <row r="11" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
+      <c r="A11" s="44">
         <v>2.2000000000000002</v>
       </c>
       <c r="B11" s="33">
         <v>1</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="32" t="s">
-        <v>87</v>
-      </c>
       <c r="I11" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
+      <c r="A12" s="44">
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" s="33">
         <v>1</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G12" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="I12" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="45">
+      <c r="A13" s="44">
         <v>2.4</v>
       </c>
       <c r="B13" s="33">
         <v>1</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="I13" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="I13" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+      <c r="A14" s="44">
         <v>2.5</v>
       </c>
       <c r="B14" s="33">
         <v>1</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="I14" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K14" s="33"/>
       <c r="L14" s="33"/>
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
+      <c r="A15" s="44">
         <v>3</v>
       </c>
       <c r="B15" s="33">
         <v>1</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="H15" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="32" t="s">
+      <c r="I15" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="42" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="34"/>
       <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
+      <c r="A16" s="44">
         <v>4</v>
       </c>
       <c r="B16" s="33">
         <v>1</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="H16" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="45">
+      <c r="A17" s="44">
         <v>4.0999999999999996</v>
       </c>
       <c r="B17" s="33">
         <v>1</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G17" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="I17" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J17" s="38" t="s">
+      <c r="J17" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K17" s="34"/>
       <c r="L17" s="33"/>
     </row>
     <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="A18" s="44">
         <v>4.2</v>
       </c>
       <c r="B18" s="33">
         <v>1</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="I18" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K18" s="34"/>
       <c r="L18" s="33"/>
     </row>
     <row r="19" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
+      <c r="A19" s="44">
         <v>4.3</v>
       </c>
       <c r="B19" s="33">
         <v>1</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="I19" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="I19" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K19" s="34"/>
       <c r="L19" s="33"/>
     </row>
     <row r="20" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="45">
+      <c r="A20" s="44">
         <v>4.4000000000000004</v>
       </c>
       <c r="B20" s="33">
         <v>1</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="I20" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="L20" s="33"/>
+        <v>124</v>
+      </c>
+      <c r="L20" s="33" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="45">
+      <c r="A21" s="44">
         <v>4.5</v>
       </c>
       <c r="B21" s="33">
         <v>1</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G21" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="I21" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="I21" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="L21" s="33"/>
+        <v>125</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="45">
+      <c r="A22" s="44">
         <v>4.5999999999999996</v>
       </c>
       <c r="B22" s="33">
         <v>1</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G22" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="I22" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="I22" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="38" t="s">
+      <c r="J22" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
     </row>
     <row r="23" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="45">
+      <c r="A23" s="44">
         <v>5</v>
       </c>
       <c r="B23" s="33">
         <v>1</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="H23" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H23" s="32" t="s">
-        <v>112</v>
-      </c>
       <c r="I23" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="J23" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" s="42" t="s">
         <v>26</v>
       </c>
       <c r="K23" s="34"/>
       <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="45">
+      <c r="A24" s="44">
         <v>6</v>
       </c>
       <c r="B24" s="33">
         <v>1</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="H24" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="I24" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="I24" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
     </row>
     <row r="25" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A25" s="45">
+      <c r="A25" s="44">
         <v>6.1</v>
       </c>
       <c r="B25" s="33">
         <v>1</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G25" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="I25" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="I25" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K25" s="34"/>
       <c r="L25" s="33"/>
     </row>
     <row r="26" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="45">
+      <c r="A26" s="44">
         <v>6.2</v>
       </c>
       <c r="B26" s="33">
         <v>1</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G26" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="I26" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="J26" s="39" t="s">
+      <c r="J26" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K26" s="34"/>
       <c r="L26" s="33"/>
     </row>
     <row r="27" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A27" s="45">
+      <c r="A27" s="44">
         <v>6.3</v>
       </c>
       <c r="B27" s="33">
         <v>1</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G27" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="I27" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="I27" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="38" t="s">
         <v>26</v>
       </c>
       <c r="K27" s="34"/>
       <c r="L27" s="33"/>
     </row>
     <row r="28" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="45">
+      <c r="A28" s="44">
         <v>6.4</v>
       </c>
       <c r="B28" s="33">
         <v>1</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G28" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="I28" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="J28" s="39" t="s">
+      <c r="J28" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="L28" s="33"/>
+        <v>142</v>
+      </c>
+      <c r="L28" s="33" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="45">
+      <c r="A29" s="44">
         <v>6.5</v>
       </c>
       <c r="B29" s="33">
         <v>1</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G29" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="I29" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="I29" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="J29" s="39" t="s">
+      <c r="J29" s="38" t="s">
         <v>31</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="L29" s="33"/>
+        <v>143</v>
+      </c>
+      <c r="L29" s="33" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="45">
+      <c r="A30" s="44">
         <v>6.6</v>
       </c>
       <c r="B30" s="33">
         <v>1</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="I30" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="I30" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="J30" s="38" t="s">
+      <c r="J30" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K30" s="33"/>
       <c r="L30" s="33"/>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="45">
+      <c r="A31" s="44">
         <v>7</v>
       </c>
       <c r="B31" s="33">
         <v>1</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="I31" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="I31" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="J31" s="38" t="s">
+      <c r="J31" s="37" t="s">
         <v>26</v>
       </c>
       <c r="K31" s="33"/>
       <c r="L31" s="33"/>
     </row>
     <row r="32" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="45">
+      <c r="A32" s="44">
         <v>7.1</v>
       </c>
       <c r="B32" s="33">
         <v>1</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F32" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="H32" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="I32" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="I32" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="J32" s="38" t="s">
+      <c r="J32" s="37" t="s">
         <v>31</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="L32" s="33"/>
-    </row>
-    <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="45">
+        <v>144</v>
+      </c>
+      <c r="L32" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="77">
         <v>8</v>
       </c>
       <c r="B33" s="33">
         <v>1</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="K33" s="34"/>
+      <c r="F33" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="J33" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="33"/>
       <c r="L33" s="33"/>
     </row>
-    <row r="34" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="45">
-        <v>9</v>
-      </c>
-      <c r="B34" s="33">
+    <row r="34" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="77">
+        <v>8.1</v>
+      </c>
+      <c r="B34" s="78">
         <v>1</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>152</v>
+      <c r="F34" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="76" t="s">
+        <v>176</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="J34" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-    </row>
-    <row r="35" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="45">
-        <v>9.1</v>
+        <v>180</v>
+      </c>
+      <c r="J34" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="L34" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="44">
+        <v>9</v>
       </c>
       <c r="B35" s="33">
         <v>1</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="J35" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="J35" s="46" t="s">
         <v>26</v>
       </c>
       <c r="K35" s="33"/>
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="45">
-        <v>9.1999999999999993</v>
+    <row r="36" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="44">
+        <v>9.1</v>
       </c>
       <c r="B36" s="33">
         <v>1</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G36" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="H36" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="I36" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="J36" s="47" t="s">
-        <v>31</v>
+      <c r="J36" s="38" t="s">
+        <v>26</v>
       </c>
       <c r="K36" s="33"/>
       <c r="L36" s="33"/>
     </row>
-    <row r="37" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="45">
-        <v>9.3000000000000007</v>
+    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="44">
+        <v>9.1999999999999993</v>
       </c>
       <c r="B37" s="33">
         <v>1</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H37" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="I37" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="I37" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="J37" s="39" t="s">
+      <c r="J37" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-    </row>
-    <row r="38" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A38" s="45">
-        <v>9.4</v>
+      <c r="K37" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="L37" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="44">
+        <v>9.3000000000000007</v>
       </c>
       <c r="B38" s="33">
         <v>1</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="G38" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="J38" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="J38" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-    </row>
-    <row r="39" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="45">
-        <v>9.5</v>
+      <c r="K38" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="L38" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="44">
+        <v>9.4</v>
       </c>
       <c r="B39" s="33">
         <v>1</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E39" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H39" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="I39" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="I39" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="J39" s="39" t="s">
+      <c r="J39" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-    </row>
-    <row r="40" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="45">
-        <v>9.6</v>
+      <c r="K39" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="L39" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="44">
+        <v>9.5</v>
       </c>
       <c r="B40" s="33">
         <v>1</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>79</v>
+        <v>166</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>145</v>
       </c>
       <c r="E40" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J40" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
+      <c r="K40" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="L40" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="44">
+        <v>9.6</v>
+      </c>
+      <c r="B41" s="33">
+        <v>1</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K41" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="L41" s="34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="77">
+        <v>10</v>
+      </c>
+      <c r="B42" s="75">
+        <v>1</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="I42" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="J42" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K42" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="L42" s="34" t="s">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3665,114 +3870,125 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="J1:J4 J6:J16 J33:J35 J40">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Invalid Test">
+  <conditionalFormatting sqref="J1:J4 J6:J16 J41 J33:J36">
+    <cfRule type="containsText" dxfId="32" priority="49" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="31" priority="50" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="30" priority="51" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="29" priority="46" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="28" priority="47" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="27" priority="48" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:J22">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="26" priority="43" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="25" priority="44" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="24" priority="45" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="23" priority="40" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="22" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="21" priority="42" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="20" priority="34" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="18" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:J32">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Invalid Test">
+  <conditionalFormatting sqref="J25:J33">
+    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J25)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Invalid Test">
-      <formula>NOT(ISERROR(SEARCH("Invalid Test",J36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",J36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",J36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J37">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="14" priority="28" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="12" priority="30" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="11" priority="25" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="26" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="9" priority="27" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:J41">
+    <cfRule type="containsText" dxfId="5" priority="19" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="20" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>